<commit_message>
fixed and finished tornado plots
* played around with the input values so that bars are same order of magnitude
</commit_message>
<xml_diff>
--- a/inst/extdata/scenario_input_values_QFT.xlsx
+++ b/inst/extdata/scenario_input_values_QFT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\R\LTBIdiagTST\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n8tha\Documents\R\LTBIdiagTST\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98A3FB5-55E4-4151-AC6E-3DD0A0A6CDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEB1807-BCC9-4CFC-AEF6-ABD87F03D2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9765" yWindow="2235" windowWidth="17040" windowHeight="13110" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>scenario</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>QFT_pos</t>
+  </si>
+  <si>
+    <t>TST</t>
+  </si>
+  <si>
+    <t>TST_pos</t>
+  </si>
+  <si>
+    <t>PPV_TST</t>
+  </si>
+  <si>
+    <t>NPV_TST</t>
   </si>
 </sst>
 </file>
@@ -635,9 +647,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -675,7 +687,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -781,7 +793,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -923,7 +935,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -951,10 +963,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,13 +982,15 @@
     <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1011,22 +1025,34 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1061,22 +1087,34 @@
         <v>23.68</v>
       </c>
       <c r="L2">
+        <v>25</v>
+      </c>
+      <c r="M2">
         <v>0.23</v>
       </c>
-      <c r="M2">
+      <c r="N2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O2">
         <v>732</v>
       </c>
-      <c r="N2">
-        <v>0.9</v>
-      </c>
-      <c r="O2">
+      <c r="P2">
+        <v>0.9</v>
+      </c>
+      <c r="Q2">
         <v>0.93</v>
       </c>
-      <c r="P2">
+      <c r="R2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S2">
+        <v>0.82</v>
+      </c>
+      <c r="T2">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1113,35 +1151,47 @@
         <v>23.68</v>
       </c>
       <c r="L3">
+        <v>25</v>
+      </c>
+      <c r="M3">
         <v>0.23</v>
       </c>
-      <c r="M3">
+      <c r="N3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O3">
         <v>732</v>
       </c>
-      <c r="N3">
-        <v>0.9</v>
-      </c>
-      <c r="O3">
+      <c r="P3">
+        <v>0.9</v>
+      </c>
+      <c r="Q3">
         <v>0.93</v>
       </c>
-      <c r="P3">
+      <c r="R3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S3">
+        <v>0.82</v>
+      </c>
+      <c r="T3">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>3.3999999999999998E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="C4" s="3">
         <f>B4*(1-0.65)</f>
-        <v>1.1899999999999999E-3</v>
+        <v>7.6999999999999996E-4</v>
       </c>
       <c r="D4" s="3">
         <f>B4*(1-0.21)</f>
-        <v>2.686E-3</v>
+        <v>1.7380000000000002E-3</v>
       </c>
       <c r="E4">
         <v>2E-3</v>
@@ -1165,22 +1215,34 @@
         <v>23.68</v>
       </c>
       <c r="L4">
+        <v>25</v>
+      </c>
+      <c r="M4">
         <v>0.23</v>
       </c>
-      <c r="M4">
+      <c r="N4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O4">
         <v>732</v>
       </c>
-      <c r="N4">
-        <v>0.9</v>
-      </c>
-      <c r="O4">
+      <c r="P4">
+        <v>0.9</v>
+      </c>
+      <c r="Q4">
         <v>0.93</v>
       </c>
-      <c r="P4">
+      <c r="R4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S4">
+        <v>0.82</v>
+      </c>
+      <c r="T4">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1215,22 +1277,34 @@
         <v>23.68</v>
       </c>
       <c r="L5">
+        <v>25</v>
+      </c>
+      <c r="M5">
         <v>0.23</v>
       </c>
-      <c r="M5">
+      <c r="N5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O5">
         <v>732</v>
       </c>
-      <c r="N5">
-        <v>0.9</v>
-      </c>
-      <c r="O5">
+      <c r="P5">
+        <v>0.9</v>
+      </c>
+      <c r="Q5">
         <v>0.93</v>
       </c>
-      <c r="P5">
+      <c r="R5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S5">
+        <v>0.82</v>
+      </c>
+      <c r="T5">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1265,22 +1339,34 @@
         <v>23.68</v>
       </c>
       <c r="L6">
+        <v>25</v>
+      </c>
+      <c r="M6">
         <v>0.23</v>
       </c>
-      <c r="M6">
+      <c r="N6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O6">
         <v>732</v>
       </c>
-      <c r="N6">
-        <v>0.9</v>
-      </c>
-      <c r="O6">
+      <c r="P6">
+        <v>0.9</v>
+      </c>
+      <c r="Q6">
         <v>0.93</v>
       </c>
-      <c r="P6">
+      <c r="R6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S6">
+        <v>0.82</v>
+      </c>
+      <c r="T6">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1315,22 +1401,34 @@
         <v>23.68</v>
       </c>
       <c r="L7">
+        <v>25</v>
+      </c>
+      <c r="M7">
         <v>0.23</v>
       </c>
-      <c r="M7">
+      <c r="N7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O7">
         <v>732</v>
       </c>
-      <c r="N7">
-        <v>0.9</v>
-      </c>
-      <c r="O7">
+      <c r="P7">
+        <v>0.9</v>
+      </c>
+      <c r="Q7">
         <v>0.93</v>
       </c>
-      <c r="P7">
+      <c r="R7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S7">
+        <v>0.82</v>
+      </c>
+      <c r="T7">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1365,22 +1463,34 @@
         <v>23.68</v>
       </c>
       <c r="L8">
+        <v>25</v>
+      </c>
+      <c r="M8">
         <v>0.23</v>
       </c>
-      <c r="M8">
+      <c r="N8">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O8">
         <v>732</v>
       </c>
-      <c r="N8">
-        <v>0.9</v>
-      </c>
-      <c r="O8">
+      <c r="P8">
+        <v>0.9</v>
+      </c>
+      <c r="Q8">
         <v>0.93</v>
       </c>
-      <c r="P8">
+      <c r="R8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S8">
+        <v>0.82</v>
+      </c>
+      <c r="T8">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1415,22 +1525,34 @@
         <v>23.68</v>
       </c>
       <c r="L9">
+        <v>25</v>
+      </c>
+      <c r="M9">
         <v>0.23</v>
       </c>
-      <c r="M9">
+      <c r="N9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O9">
         <v>732</v>
       </c>
-      <c r="N9" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="O9">
+      <c r="P9" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="Q9">
         <v>0.93</v>
       </c>
-      <c r="P9">
+      <c r="R9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S9">
+        <v>0.82</v>
+      </c>
+      <c r="T9">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1465,22 +1587,34 @@
         <v>23.68</v>
       </c>
       <c r="L10">
+        <v>25</v>
+      </c>
+      <c r="M10">
         <v>0.23</v>
       </c>
-      <c r="M10">
+      <c r="N10">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O10">
         <v>732</v>
       </c>
-      <c r="N10" s="2">
+      <c r="P10" s="2">
         <v>1</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>0.93</v>
       </c>
-      <c r="P10">
+      <c r="R10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S10">
+        <v>0.82</v>
+      </c>
+      <c r="T10">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1515,22 +1649,34 @@
         <v>23.68</v>
       </c>
       <c r="L11">
+        <v>25</v>
+      </c>
+      <c r="M11">
         <v>0.23</v>
       </c>
-      <c r="M11">
+      <c r="N11">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O11">
         <v>732</v>
       </c>
-      <c r="N11">
-        <v>0.9</v>
-      </c>
-      <c r="O11">
+      <c r="P11">
+        <v>0.9</v>
+      </c>
+      <c r="Q11">
         <v>0.93</v>
       </c>
-      <c r="P11">
+      <c r="R11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S11">
+        <v>0.82</v>
+      </c>
+      <c r="T11">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1565,22 +1711,34 @@
         <v>23.68</v>
       </c>
       <c r="L12">
+        <v>25</v>
+      </c>
+      <c r="M12">
         <v>0.23</v>
       </c>
-      <c r="M12">
+      <c r="N12">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O12">
         <v>732</v>
       </c>
-      <c r="N12">
-        <v>0.9</v>
-      </c>
-      <c r="O12">
+      <c r="P12">
+        <v>0.9</v>
+      </c>
+      <c r="Q12">
         <v>0.93</v>
       </c>
-      <c r="P12">
+      <c r="R12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S12">
+        <v>0.82</v>
+      </c>
+      <c r="T12">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1615,22 +1773,34 @@
         <v>23.68</v>
       </c>
       <c r="L13">
+        <v>25</v>
+      </c>
+      <c r="M13">
         <v>0.23</v>
       </c>
-      <c r="M13">
+      <c r="N13">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O13">
         <v>732</v>
       </c>
-      <c r="N13">
-        <v>0.9</v>
-      </c>
-      <c r="O13">
+      <c r="P13">
+        <v>0.9</v>
+      </c>
+      <c r="Q13">
         <v>0.93</v>
       </c>
-      <c r="P13">
+      <c r="R13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S13">
+        <v>0.82</v>
+      </c>
+      <c r="T13">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1665,22 +1835,34 @@
         <v>23.68</v>
       </c>
       <c r="L14">
+        <v>25</v>
+      </c>
+      <c r="M14">
         <v>0.23</v>
       </c>
-      <c r="M14">
+      <c r="N14">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O14">
         <v>732</v>
       </c>
-      <c r="N14">
-        <v>0.9</v>
-      </c>
-      <c r="O14">
+      <c r="P14">
+        <v>0.9</v>
+      </c>
+      <c r="Q14">
         <v>0.93</v>
       </c>
-      <c r="P14">
+      <c r="R14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S14">
+        <v>0.82</v>
+      </c>
+      <c r="T14">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1715,22 +1897,34 @@
         <v>23.68</v>
       </c>
       <c r="L15">
+        <v>25</v>
+      </c>
+      <c r="M15">
         <v>0.23</v>
       </c>
-      <c r="M15">
+      <c r="N15">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O15">
         <v>732</v>
       </c>
-      <c r="N15">
-        <v>0.9</v>
-      </c>
-      <c r="O15">
+      <c r="P15">
+        <v>0.9</v>
+      </c>
+      <c r="Q15">
         <v>0.93</v>
       </c>
-      <c r="P15">
+      <c r="R15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S15">
+        <v>0.82</v>
+      </c>
+      <c r="T15">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1765,22 +1959,34 @@
         <v>23.68</v>
       </c>
       <c r="L16">
+        <v>25</v>
+      </c>
+      <c r="M16">
         <v>0.23</v>
       </c>
-      <c r="M16">
+      <c r="N16">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O16">
         <v>732</v>
       </c>
-      <c r="N16">
-        <v>0.9</v>
-      </c>
-      <c r="O16">
+      <c r="P16">
+        <v>0.9</v>
+      </c>
+      <c r="Q16">
         <v>0.93</v>
       </c>
-      <c r="P16">
+      <c r="R16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S16">
+        <v>0.82</v>
+      </c>
+      <c r="T16">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1815,22 +2021,34 @@
         <v>23.68</v>
       </c>
       <c r="L17">
+        <v>25</v>
+      </c>
+      <c r="M17">
         <v>0.23</v>
       </c>
-      <c r="M17">
+      <c r="N17">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O17">
         <v>732</v>
       </c>
-      <c r="N17">
-        <v>0.9</v>
-      </c>
-      <c r="O17">
+      <c r="P17">
+        <v>0.9</v>
+      </c>
+      <c r="Q17">
         <v>0.93</v>
       </c>
-      <c r="P17">
+      <c r="R17">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S17">
+        <v>0.82</v>
+      </c>
+      <c r="T17">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1865,22 +2083,34 @@
         <v>23.68</v>
       </c>
       <c r="L18">
+        <v>25</v>
+      </c>
+      <c r="M18">
         <v>0.23</v>
       </c>
-      <c r="M18">
+      <c r="N18">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O18">
         <v>732</v>
       </c>
-      <c r="N18">
-        <v>0.9</v>
-      </c>
-      <c r="O18">
+      <c r="P18">
+        <v>0.9</v>
+      </c>
+      <c r="Q18">
         <v>0.93</v>
       </c>
-      <c r="P18">
+      <c r="R18">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S18">
+        <v>0.82</v>
+      </c>
+      <c r="T18">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1915,22 +2145,34 @@
         <v>10</v>
       </c>
       <c r="L19">
+        <v>25</v>
+      </c>
+      <c r="M19">
         <v>0.23</v>
       </c>
-      <c r="M19">
+      <c r="N19">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O19">
         <v>732</v>
       </c>
-      <c r="N19">
-        <v>0.9</v>
-      </c>
-      <c r="O19">
+      <c r="P19">
+        <v>0.9</v>
+      </c>
+      <c r="Q19">
         <v>0.93</v>
       </c>
-      <c r="P19">
+      <c r="R19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S19">
+        <v>0.82</v>
+      </c>
+      <c r="T19">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1965,22 +2207,34 @@
         <v>100</v>
       </c>
       <c r="L20">
+        <v>25</v>
+      </c>
+      <c r="M20">
         <v>0.23</v>
       </c>
-      <c r="M20">
+      <c r="N20">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O20">
         <v>732</v>
       </c>
-      <c r="N20">
-        <v>0.9</v>
-      </c>
-      <c r="O20">
+      <c r="P20">
+        <v>0.9</v>
+      </c>
+      <c r="Q20">
         <v>0.93</v>
       </c>
-      <c r="P20">
+      <c r="R20">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S20">
+        <v>0.82</v>
+      </c>
+      <c r="T20">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2014,23 +2268,35 @@
       <c r="K21">
         <v>23.68</v>
       </c>
-      <c r="L21" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="M21">
+      <c r="L21">
+        <v>25</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="N21">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O21">
         <v>732</v>
       </c>
-      <c r="N21">
-        <v>0.9</v>
-      </c>
-      <c r="O21">
+      <c r="P21">
+        <v>0.9</v>
+      </c>
+      <c r="Q21">
         <v>0.93</v>
       </c>
-      <c r="P21">
+      <c r="R21">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S21">
+        <v>0.82</v>
+      </c>
+      <c r="T21">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2064,23 +2330,35 @@
       <c r="K22">
         <v>23.68</v>
       </c>
-      <c r="L22" s="2">
-        <v>0.26</v>
-      </c>
-      <c r="M22">
+      <c r="L22">
+        <v>25</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="N22">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O22">
         <v>732</v>
       </c>
-      <c r="N22">
-        <v>0.9</v>
-      </c>
-      <c r="O22">
+      <c r="P22">
+        <v>0.9</v>
+      </c>
+      <c r="Q22">
         <v>0.93</v>
       </c>
-      <c r="P22">
+      <c r="R22">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S22">
+        <v>0.82</v>
+      </c>
+      <c r="T22">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2115,22 +2393,34 @@
         <v>23.68</v>
       </c>
       <c r="L23">
+        <v>25</v>
+      </c>
+      <c r="M23">
         <v>0.23</v>
       </c>
-      <c r="M23" s="2">
+      <c r="N23">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O23" s="2">
         <v>366</v>
       </c>
-      <c r="N23">
-        <v>0.9</v>
-      </c>
-      <c r="O23">
+      <c r="P23">
+        <v>0.9</v>
+      </c>
+      <c r="Q23">
         <v>0.93</v>
       </c>
-      <c r="P23">
+      <c r="R23">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S23">
+        <v>0.82</v>
+      </c>
+      <c r="T23">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2165,22 +2455,34 @@
         <v>23.68</v>
       </c>
       <c r="L24">
+        <v>25</v>
+      </c>
+      <c r="M24">
         <v>0.23</v>
       </c>
-      <c r="M24" s="2">
+      <c r="N24">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O24" s="2">
         <v>1464</v>
       </c>
-      <c r="N24">
-        <v>0.9</v>
-      </c>
-      <c r="O24">
+      <c r="P24">
+        <v>0.9</v>
+      </c>
+      <c r="Q24">
         <v>0.93</v>
       </c>
-      <c r="P24">
+      <c r="R24">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S24">
+        <v>0.82</v>
+      </c>
+      <c r="T24">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2215,22 +2517,34 @@
         <v>23.68</v>
       </c>
       <c r="L25">
+        <v>25</v>
+      </c>
+      <c r="M25">
         <v>0.23</v>
       </c>
-      <c r="M25">
+      <c r="N25">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O25">
         <v>732</v>
       </c>
-      <c r="N25">
-        <v>0.9</v>
-      </c>
-      <c r="O25" s="2">
-        <v>0.8</v>
-      </c>
       <c r="P25">
+        <v>0.9</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="R25">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S25">
+        <v>0.82</v>
+      </c>
+      <c r="T25">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2265,22 +2579,34 @@
         <v>23.68</v>
       </c>
       <c r="L26">
+        <v>25</v>
+      </c>
+      <c r="M26">
         <v>0.23</v>
       </c>
-      <c r="M26">
+      <c r="N26">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O26">
         <v>732</v>
       </c>
-      <c r="N26">
-        <v>0.9</v>
-      </c>
-      <c r="O26" s="2">
+      <c r="P26">
+        <v>0.9</v>
+      </c>
+      <c r="Q26" s="2">
         <v>1</v>
       </c>
-      <c r="P26">
+      <c r="R26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S26">
+        <v>0.82</v>
+      </c>
+      <c r="T26">
         <v>4925.76</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2315,22 +2641,34 @@
         <v>23.68</v>
       </c>
       <c r="L27">
+        <v>25</v>
+      </c>
+      <c r="M27">
         <v>0.23</v>
       </c>
-      <c r="M27">
+      <c r="N27">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O27">
         <v>732</v>
       </c>
-      <c r="N27">
-        <v>0.9</v>
-      </c>
-      <c r="O27">
+      <c r="P27">
+        <v>0.9</v>
+      </c>
+      <c r="Q27">
         <v>0.93</v>
       </c>
-      <c r="P27" s="2">
+      <c r="R27">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S27">
+        <v>0.82</v>
+      </c>
+      <c r="T27" s="2">
         <v>2463</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2365,19 +2703,527 @@
         <v>23.68</v>
       </c>
       <c r="L28">
+        <v>25</v>
+      </c>
+      <c r="M28">
         <v>0.23</v>
       </c>
-      <c r="M28">
+      <c r="N28">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O28">
         <v>732</v>
       </c>
-      <c r="N28">
-        <v>0.9</v>
-      </c>
-      <c r="O28">
+      <c r="P28">
+        <v>0.9</v>
+      </c>
+      <c r="Q28">
         <v>0.93</v>
       </c>
-      <c r="P28" s="2">
+      <c r="R28">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S28">
+        <v>0.82</v>
+      </c>
+      <c r="T28" s="2">
         <v>9851</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="C29">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D29">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E29">
+        <v>2E-3</v>
+      </c>
+      <c r="F29">
+        <v>0.8</v>
+      </c>
+      <c r="G29">
+        <v>241.23</v>
+      </c>
+      <c r="H29">
+        <v>169.68</v>
+      </c>
+      <c r="I29">
+        <v>84.84</v>
+      </c>
+      <c r="J29">
+        <v>0.95</v>
+      </c>
+      <c r="K29">
+        <v>23.68</v>
+      </c>
+      <c r="L29" s="2">
+        <v>12</v>
+      </c>
+      <c r="M29">
+        <v>0.23</v>
+      </c>
+      <c r="N29">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O29">
+        <v>732</v>
+      </c>
+      <c r="P29">
+        <v>0.9</v>
+      </c>
+      <c r="Q29">
+        <v>0.93</v>
+      </c>
+      <c r="R29">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S29">
+        <v>0.82</v>
+      </c>
+      <c r="T29">
+        <v>4925.76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="C30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D30">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E30">
+        <v>2E-3</v>
+      </c>
+      <c r="F30">
+        <v>0.8</v>
+      </c>
+      <c r="G30">
+        <v>241.23</v>
+      </c>
+      <c r="H30">
+        <v>169.68</v>
+      </c>
+      <c r="I30">
+        <v>84.84</v>
+      </c>
+      <c r="J30">
+        <v>0.95</v>
+      </c>
+      <c r="K30">
+        <v>23.68</v>
+      </c>
+      <c r="L30" s="2">
+        <v>50</v>
+      </c>
+      <c r="M30">
+        <v>0.23</v>
+      </c>
+      <c r="N30">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O30">
+        <v>732</v>
+      </c>
+      <c r="P30">
+        <v>0.9</v>
+      </c>
+      <c r="Q30">
+        <v>0.93</v>
+      </c>
+      <c r="R30">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S30">
+        <v>0.82</v>
+      </c>
+      <c r="T30">
+        <v>4925.76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="C31">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D31">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E31">
+        <v>2E-3</v>
+      </c>
+      <c r="F31">
+        <v>0.8</v>
+      </c>
+      <c r="G31">
+        <v>241.23</v>
+      </c>
+      <c r="H31">
+        <v>169.68</v>
+      </c>
+      <c r="I31">
+        <v>84.84</v>
+      </c>
+      <c r="J31">
+        <v>0.95</v>
+      </c>
+      <c r="K31">
+        <v>23.68</v>
+      </c>
+      <c r="L31">
+        <v>25</v>
+      </c>
+      <c r="M31">
+        <v>0.23</v>
+      </c>
+      <c r="N31" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="O31">
+        <v>732</v>
+      </c>
+      <c r="P31">
+        <v>0.9</v>
+      </c>
+      <c r="Q31">
+        <v>0.93</v>
+      </c>
+      <c r="R31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S31">
+        <v>0.82</v>
+      </c>
+      <c r="T31">
+        <v>4925.76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="C32">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D32">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E32">
+        <v>2E-3</v>
+      </c>
+      <c r="F32">
+        <v>0.8</v>
+      </c>
+      <c r="G32">
+        <v>241.23</v>
+      </c>
+      <c r="H32">
+        <v>169.68</v>
+      </c>
+      <c r="I32">
+        <v>84.84</v>
+      </c>
+      <c r="J32">
+        <v>0.95</v>
+      </c>
+      <c r="K32">
+        <v>23.68</v>
+      </c>
+      <c r="L32">
+        <v>25</v>
+      </c>
+      <c r="M32">
+        <v>0.23</v>
+      </c>
+      <c r="N32" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O32">
+        <v>732</v>
+      </c>
+      <c r="P32">
+        <v>0.9</v>
+      </c>
+      <c r="Q32">
+        <v>0.93</v>
+      </c>
+      <c r="R32">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S32">
+        <v>0.82</v>
+      </c>
+      <c r="T32">
+        <v>4925.76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="C33">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D33">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E33">
+        <v>2E-3</v>
+      </c>
+      <c r="F33">
+        <v>0.8</v>
+      </c>
+      <c r="G33">
+        <v>241.23</v>
+      </c>
+      <c r="H33">
+        <v>169.68</v>
+      </c>
+      <c r="I33">
+        <v>84.84</v>
+      </c>
+      <c r="J33">
+        <v>0.95</v>
+      </c>
+      <c r="K33">
+        <v>23.68</v>
+      </c>
+      <c r="L33">
+        <v>25</v>
+      </c>
+      <c r="M33">
+        <v>0.23</v>
+      </c>
+      <c r="N33">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O33">
+        <v>732</v>
+      </c>
+      <c r="P33">
+        <v>0.9</v>
+      </c>
+      <c r="Q33">
+        <v>0.93</v>
+      </c>
+      <c r="R33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="S33">
+        <v>0.82</v>
+      </c>
+      <c r="T33">
+        <v>4925.76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="C34">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D34">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E34">
+        <v>2E-3</v>
+      </c>
+      <c r="F34">
+        <v>0.8</v>
+      </c>
+      <c r="G34">
+        <v>241.23</v>
+      </c>
+      <c r="H34">
+        <v>169.68</v>
+      </c>
+      <c r="I34">
+        <v>84.84</v>
+      </c>
+      <c r="J34">
+        <v>0.95</v>
+      </c>
+      <c r="K34">
+        <v>23.68</v>
+      </c>
+      <c r="L34">
+        <v>25</v>
+      </c>
+      <c r="M34">
+        <v>0.23</v>
+      </c>
+      <c r="N34">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O34">
+        <v>732</v>
+      </c>
+      <c r="P34">
+        <v>0.9</v>
+      </c>
+      <c r="Q34">
+        <v>0.93</v>
+      </c>
+      <c r="R34" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="S34">
+        <v>0.82</v>
+      </c>
+      <c r="T34">
+        <v>4925.76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="C35">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D35">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E35">
+        <v>2E-3</v>
+      </c>
+      <c r="F35">
+        <v>0.8</v>
+      </c>
+      <c r="G35">
+        <v>241.23</v>
+      </c>
+      <c r="H35">
+        <v>169.68</v>
+      </c>
+      <c r="I35">
+        <v>84.84</v>
+      </c>
+      <c r="J35">
+        <v>0.95</v>
+      </c>
+      <c r="K35">
+        <v>23.68</v>
+      </c>
+      <c r="L35">
+        <v>25</v>
+      </c>
+      <c r="M35">
+        <v>0.23</v>
+      </c>
+      <c r="N35">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O35">
+        <v>732</v>
+      </c>
+      <c r="P35">
+        <v>0.9</v>
+      </c>
+      <c r="Q35">
+        <v>0.93</v>
+      </c>
+      <c r="R35">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S35" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="T35">
+        <v>4925.76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="C36">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D36">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E36">
+        <v>2E-3</v>
+      </c>
+      <c r="F36">
+        <v>0.8</v>
+      </c>
+      <c r="G36">
+        <v>241.23</v>
+      </c>
+      <c r="H36">
+        <v>169.68</v>
+      </c>
+      <c r="I36">
+        <v>84.84</v>
+      </c>
+      <c r="J36">
+        <v>0.95</v>
+      </c>
+      <c r="K36">
+        <v>23.68</v>
+      </c>
+      <c r="L36">
+        <v>25</v>
+      </c>
+      <c r="M36">
+        <v>0.23</v>
+      </c>
+      <c r="N36">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O36">
+        <v>732</v>
+      </c>
+      <c r="P36">
+        <v>0.9</v>
+      </c>
+      <c r="Q36">
+        <v>0.93</v>
+      </c>
+      <c r="R36">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S36" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="T36">
+        <v>4925.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>